<commit_message>
pushing data provider test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kisho\eclipse-workspace\TestNgFrameWorkProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED18C40-B579-4FC9-8340-9A3F84E3E1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD830DE-07F9-4D1A-99E9-746434F73FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5461AA17-FD0E-4CC1-AC77-336A09AB42A6}"/>
   </bookViews>
   <sheets>
     <sheet name="test01" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>https://www.facebook.com/</t>
   </si>
@@ -50,13 +49,16 @@
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,12 +73,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,13 +96,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -422,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C183B29D-F120-482E-BAC5-D8493F3C97E2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,7 +429,7 @@
     <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -459,13 +452,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -476,20 +480,12 @@
     <hyperlink ref="B3" r:id="rId3" xr:uid="{D58102F1-5614-4753-BCBA-167227EFBF61}"/>
     <hyperlink ref="C2" r:id="rId4" xr:uid="{EE548ED5-FFF6-44EF-ADD6-18345B4E15C9}"/>
     <hyperlink ref="C3" r:id="rId5" xr:uid="{CD42780B-A01C-42BF-8574-07630B58548D}"/>
+    <hyperlink ref="A3" r:id="rId6" xr:uid="{C46939A7-4179-43E0-8133-CDD7D8E3F0A9}"/>
+    <hyperlink ref="B4" r:id="rId7" display="test@gmail.com" xr:uid="{5C8C1549-05A7-406D-85A5-755330A21072}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{9FCA395A-BFC5-4D83-A414-1A2EC89A0448}"/>
+    <hyperlink ref="A4" r:id="rId9" xr:uid="{E5E33510-4EE2-442E-82C4-F3BFD7C51865}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC5AF25-B916-47B1-8480-C99A7FDB0464}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>